<commit_message>
VM for searching people added
</commit_message>
<xml_diff>
--- a/ExcelWorkerTests/Resources/ImportPeople_template.xlsx
+++ b/ExcelWorkerTests/Resources/ImportPeople_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artem.kiyashko\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artem.kiyashko\Documents\Visual Studio 2017\Projects\AmSpaceTools\ExcelWorkerTests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,9 +53,6 @@
     <t>Sex</t>
   </si>
   <si>
-    <t>EmployeeId</t>
-  </si>
-  <si>
     <t>ContractNumber</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>AISHAT</t>
   </si>
   <si>
-    <t>ARF 123 789</t>
-  </si>
-  <si>
     <t>mymail@mail.com</t>
   </si>
   <si>
@@ -107,9 +101,6 @@
     <t>JIHENE</t>
   </si>
   <si>
-    <t>3565 7895</t>
-  </si>
-  <si>
     <t>othermail@mail.com</t>
   </si>
   <si>
@@ -140,10 +131,19 @@
     <t>LUCAS</t>
   </si>
   <si>
-    <t>TD 346 009</t>
-  </si>
-  <si>
     <t>ADMINISTRATION COORDINATOR</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Terminated</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Suspended</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="K2" sqref="K2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,11 +537,11 @@
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="8" max="8" width="14.140625" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="11" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" customWidth="1"/>
-    <col min="14" max="14" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" style="11" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
+    <col min="13" max="13" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -570,16 +570,16 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>34</v>
       </c>
       <c r="M1" t="s">
         <v>10</v>
@@ -594,173 +594,169 @@
         <v>13</v>
       </c>
       <c r="Q1" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
+      <c r="C2" s="7">
+        <v>290109933804360</v>
       </c>
       <c r="D2" s="7">
         <v>1303012</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2">
         <v>31773</v>
       </c>
       <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" s="7"/>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2">
-        <v>322588097</v>
-      </c>
-      <c r="L2">
-        <v>569430803</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2">
+      <c r="N2">
         <v>3</v>
       </c>
+      <c r="O2" s="1">
+        <v>42478</v>
+      </c>
       <c r="P2" s="1">
-        <v>42478</v>
-      </c>
-      <c r="Q2" s="1">
         <v>43817</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
+      <c r="C3" s="7">
+        <v>290109933804360</v>
       </c>
       <c r="D3" s="7">
         <v>1303012</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G3" s="2">
         <v>31773</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="7"/>
+      <c r="L3" s="3">
+        <v>2</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K3">
-        <v>322588097</v>
-      </c>
-      <c r="L3">
-        <v>569430803</v>
-      </c>
-      <c r="M3" s="3">
-        <v>2</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="3">
+      <c r="N3" s="3">
         <v>4</v>
       </c>
-      <c r="P3" s="1">
+      <c r="O3" s="1">
         <v>43208</v>
       </c>
-      <c r="Q3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="12" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="C4" s="7">
+        <v>168039933804012</v>
       </c>
       <c r="D4" s="8">
         <v>1303026</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G4" s="2">
         <v>36537</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4">
-        <v>16071774</v>
-      </c>
-      <c r="L4" s="12">
-        <v>322588097</v>
-      </c>
-      <c r="M4" s="5">
+        <v>29</v>
+      </c>
+      <c r="K4" s="7">
+        <v>290109933804360</v>
+      </c>
+      <c r="L4" s="5">
         <v>1</v>
       </c>
-      <c r="N4" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="O4" s="5">
+      <c r="M4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="5">
         <v>1</v>
       </c>
-      <c r="P4" s="1">
+      <c r="O4" s="1">
         <v>42736</v>
       </c>
-      <c r="Q4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="C5" s="7">
+        <v>169129934203490</v>
       </c>
       <c r="D5" s="8">
         <v>1303065</v>
@@ -771,34 +767,34 @@
         <v>31764</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5">
-        <v>412589481</v>
+        <v>20</v>
+      </c>
+      <c r="K5" s="7">
+        <v>168039933804012</v>
       </c>
       <c r="L5" s="12">
-        <v>16071774</v>
-      </c>
-      <c r="M5" s="12">
         <v>1</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="M5" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="12">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>38627</v>
+      </c>
+      <c r="P5" s="1">
+        <v>43375</v>
+      </c>
+      <c r="Q5" t="s">
         <v>39</v>
-      </c>
-      <c r="O5" s="12">
-        <v>1</v>
-      </c>
-      <c r="P5" s="1">
-        <v>38627</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>43375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grouping account by identity id and manager id for attaching several contracts to one account. ImportPeople_template updated to store identity id and manager id as a text not numbers.
</commit_message>
<xml_diff>
--- a/ExcelWorkerTests/Resources/ImportPeople_template.xlsx
+++ b/ExcelWorkerTests/Resources/ImportPeople_template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -144,6 +144,24 @@
   </si>
   <si>
     <t>Suspended</t>
+  </si>
+  <si>
+    <t>AOUDI1</t>
+  </si>
+  <si>
+    <t>JIHENE1</t>
+  </si>
+  <si>
+    <t>290109933804360</t>
+  </si>
+  <si>
+    <t>168039933804012</t>
+  </si>
+  <si>
+    <t>169129934203490</t>
+  </si>
+  <si>
+    <t>1680399338040120</t>
   </si>
 </sst>
 </file>
@@ -182,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -207,6 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,16 +540,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B699643A-B2E0-47E1-AAE6-24FCF5A35A8E}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="14" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
@@ -551,7 +570,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -575,7 +594,7 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="14" t="s">
         <v>31</v>
       </c>
       <c r="L1" t="s">
@@ -604,8 +623,8 @@
       <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="7">
-        <v>290109933804360</v>
+      <c r="C2" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="D2" s="7">
         <v>1303012</v>
@@ -655,8 +674,8 @@
       <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="7">
-        <v>290109933804360</v>
+      <c r="C3" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="D3" s="7">
         <v>1303012</v>
@@ -704,8 +723,8 @@
       <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="7">
-        <v>168039933804012</v>
+      <c r="C4" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="D4" s="8">
         <v>1303026</v>
@@ -728,8 +747,8 @@
       <c r="J4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="7">
-        <v>290109933804360</v>
+      <c r="K4" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="L4" s="5">
         <v>1</v>
@@ -755,8 +774,8 @@
       <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="7">
-        <v>169129934203490</v>
+      <c r="C5" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D5" s="8">
         <v>1303065</v>
@@ -775,8 +794,8 @@
       <c r="J5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="7">
-        <v>168039933804012</v>
+      <c r="K5" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="L5" s="12">
         <v>1</v>
@@ -795,6 +814,108 @@
       </c>
       <c r="Q5" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1303026</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="2">
+        <v>36537</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="12">
+        <v>1</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="12">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
+        <v>42736</v>
+      </c>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1303026</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="2">
+        <v>36537</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="12">
+        <v>2</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="12">
+        <v>1</v>
+      </c>
+      <c r="O7" s="1">
+        <v>42736</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="12" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -802,8 +923,10 @@
     <hyperlink ref="E2" r:id="rId1" xr:uid="{0F26F954-7375-4613-8132-95076F505D8A}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{33B6039C-BB64-4441-8CB1-13BABEA3D828}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{A5A688E6-EAE5-4C5D-8603-461D16BA6B67}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{4EFDE32B-9E97-4942-9FAE-EF6A66060EA2}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{86B2F484-A451-4219-9840-CB962F8B3E53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix people template to fulfill the requirement that Email is required field
</commit_message>
<xml_diff>
--- a/ExcelWorkerTests/Resources/ImportPeople_template.xlsx
+++ b/ExcelWorkerTests/Resources/ImportPeople_template.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artem.kiyashko\Documents\Visual Studio 2017\Projects\AmSpaceTools\ExcelWorkerTests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F795B1E-5138-4B9F-847E-0065C3A1BEE8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{24A8D7F6-D52A-4993-B4D0-2FB204761490}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -543,7 +544,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,7 +781,9 @@
       <c r="D5" s="8">
         <v>1303065</v>
       </c>
-      <c r="E5" s="12"/>
+      <c r="E5" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="F5" s="9"/>
       <c r="G5" s="2">
         <v>31764</v>
@@ -925,8 +928,9 @@
     <hyperlink ref="E4" r:id="rId3" xr:uid="{A5A688E6-EAE5-4C5D-8603-461D16BA6B67}"/>
     <hyperlink ref="E6" r:id="rId4" xr:uid="{4EFDE32B-9E97-4942-9FAE-EF6A66060EA2}"/>
     <hyperlink ref="E7" r:id="rId5" xr:uid="{86B2F484-A451-4219-9840-CB962F8B3E53}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{8F8A0F45-0217-45D9-A871-FCB5D03E7FDF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added AmRest Manager Name column to people template
</commit_message>
<xml_diff>
--- a/ExcelWorkerTests/Resources/ImportPeople_template.xlsx
+++ b/ExcelWorkerTests/Resources/ImportPeople_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artem.kiyashko\Documents\Visual Studio 2017\Projects\AmSpaceTools\ExcelWorkerTests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F795B1E-5138-4B9F-847E-0065C3A1BEE8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAD6FD5-3A54-4470-9B0D-04404F1D7269}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{24A8D7F6-D52A-4993-B4D0-2FB204761490}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>1680399338040120</t>
+  </si>
+  <si>
+    <t>AmRest Manager Name</t>
   </si>
 </sst>
 </file>
@@ -541,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B699643A-B2E0-47E1-AAE6-24FCF5A35A8E}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,9 +565,10 @@
     <col min="13" max="13" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="13.28515625" customWidth="1"/>
     <col min="17" max="17" width="11.7109375" customWidth="1"/>
+    <col min="18" max="18" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -616,8 +620,11 @@
       <c r="Q1" t="s">
         <v>36</v>
       </c>
+      <c r="R1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -668,7 +675,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -717,7 +724,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -768,7 +775,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -819,7 +826,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>40</v>
       </c>
@@ -870,7 +877,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>40</v>
       </c>

</xml_diff>